<commit_message>
Updating Zoop SEM Categories, and adding Rotifers as a category
</commit_message>
<xml_diff>
--- a/data/data_in/Zoop Categories for SEM.xlsx
+++ b/data/data_in/Zoop Categories for SEM.xlsx
@@ -5,22 +5,40 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburdi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\NCEAS Working Group\Zoop Wrangling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C156DAF0-3C64-49F6-BA54-4BE0C35322E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{99D70CA2-450C-425C-BF25-7A182FB1919A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
   </bookViews>
   <sheets>
-    <sheet name="biomass_mesomicro" sheetId="1" r:id="rId1"/>
+    <sheet name="Zoop Categories for SEM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="64">
+  <si>
+    <t>SEM Category</t>
+  </si>
+  <si>
+    <t>Taxonomic Category</t>
+  </si>
+  <si>
+    <t>Trophic Category</t>
+  </si>
   <si>
     <t>Taxname</t>
   </si>
@@ -31,48 +49,87 @@
     <t>Carbon_mass_micrograms</t>
   </si>
   <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Herbivorous Copepods</t>
+  </si>
+  <si>
+    <t>Copepod Nauplii</t>
+  </si>
+  <si>
+    <t>Herbivorous</t>
+  </si>
+  <si>
+    <t>Juvenile</t>
+  </si>
+  <si>
+    <t>Predatory copepods have predatory nauplii?</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Calanoid Copepod</t>
+  </si>
+  <si>
+    <t>Acartia</t>
+  </si>
+  <si>
+    <t>Adult</t>
+  </si>
+  <si>
+    <t>Predatory Copepods</t>
+  </si>
+  <si>
+    <t>Predatory</t>
+  </si>
+  <si>
+    <t>Acartiella sinensis</t>
+  </si>
+  <si>
+    <t>Cladoceran</t>
+  </si>
+  <si>
+    <t>Bosmina longirostris</t>
+  </si>
+  <si>
+    <t>Cirripedia</t>
+  </si>
+  <si>
+    <t>Larva</t>
+  </si>
+  <si>
+    <t>Daphnia</t>
+  </si>
+  <si>
+    <t>Diaphanosoma</t>
+  </si>
+  <si>
+    <t>Diaptomidae</t>
+  </si>
+  <si>
+    <t>Eurytemora affinis</t>
+  </si>
+  <si>
+    <t>Harpacticoid</t>
+  </si>
+  <si>
+    <t>Harpacticoida</t>
+  </si>
+  <si>
+    <t>Undifferentiated</t>
+  </si>
+  <si>
+    <t>Cyclopoid</t>
+  </si>
+  <si>
+    <t>Acanthocyclops</t>
+  </si>
+  <si>
     <t>Limnoithona</t>
   </si>
   <si>
-    <t>Juvenile</t>
-  </si>
-  <si>
-    <t>Acartia</t>
-  </si>
-  <si>
-    <t>Adult</t>
-  </si>
-  <si>
-    <t>Acartiella sinensis</t>
-  </si>
-  <si>
-    <t>Bosmina longirostris</t>
-  </si>
-  <si>
-    <t>Cirripedia</t>
-  </si>
-  <si>
-    <t>Larva</t>
-  </si>
-  <si>
-    <t>Daphnia</t>
-  </si>
-  <si>
-    <t>Diaphanosoma</t>
-  </si>
-  <si>
-    <t>Diaptomidae</t>
-  </si>
-  <si>
-    <t>Eurytemora affinis</t>
-  </si>
-  <si>
-    <t>Harpacticoida</t>
-  </si>
-  <si>
-    <t>Undifferentiated</t>
-  </si>
-  <si>
     <t>Limnoithona sinensis</t>
   </si>
   <si>
@@ -103,33 +160,6 @@
     <t>Tortanus</t>
   </si>
   <si>
-    <t>Trophic Category</t>
-  </si>
-  <si>
-    <t>Herbivorous</t>
-  </si>
-  <si>
-    <t>Predatory</t>
-  </si>
-  <si>
-    <t>Taxonomic Category</t>
-  </si>
-  <si>
-    <t>Calanoid Copepod</t>
-  </si>
-  <si>
-    <t>Cladoceran</t>
-  </si>
-  <si>
-    <t>Harpacticoid</t>
-  </si>
-  <si>
-    <t>Cyclopoid</t>
-  </si>
-  <si>
-    <t>Acanthocyclops</t>
-  </si>
-  <si>
     <t>Mysids</t>
   </si>
   <si>
@@ -145,12 +175,39 @@
     <t>Omnivores, suspension feeding?</t>
   </si>
   <si>
+    <t>Rotifers</t>
+  </si>
+  <si>
+    <t>Keratella</t>
+  </si>
+  <si>
+    <t>Synchaeta</t>
+  </si>
+  <si>
+    <t>Asplanchna</t>
+  </si>
+  <si>
+    <t>Omnivorous</t>
+  </si>
+  <si>
+    <t>Trichocerca</t>
+  </si>
+  <si>
+    <t>Polyarthra</t>
+  </si>
+  <si>
+    <t>Other Rotifer</t>
+  </si>
+  <si>
     <t>Amphipods</t>
   </si>
   <si>
     <t>Gammarus daiberi</t>
   </si>
   <si>
+    <t>Use EMP benthic for amphipods, only CPUE</t>
+  </si>
+  <si>
     <t>Americorophium spinicorne</t>
   </si>
   <si>
@@ -164,24 +221,6 @@
   </si>
   <si>
     <t>Hyalella spp</t>
-  </si>
-  <si>
-    <t>SEM Category</t>
-  </si>
-  <si>
-    <t>Copepod Nauplii</t>
-  </si>
-  <si>
-    <t>Herbivorous Copepods</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Cyclopoids</t>
-  </si>
-  <si>
-    <t>Predatory Calanoids</t>
   </si>
 </sst>
 </file>
@@ -324,7 +363,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -502,12 +541,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -629,95 +662,94 @@
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="21" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="37" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="38" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="39" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1029,932 +1061,830 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.1796875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F3">
         <v>1.3009999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F4">
         <v>2.984</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F5">
         <v>1.1619999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F6">
         <v>2.6659999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F7">
         <v>0.6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F8">
         <v>3.8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F9">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F11">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F12">
         <v>1.4430000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F13">
         <v>3.55</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="E14" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F15">
         <v>3.36</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="E16" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F16">
         <v>0.13300000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E17" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F17">
         <v>0.13300000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
         <v>34</v>
       </c>
-      <c r="D18" t="s">
-        <v>18</v>
-      </c>
       <c r="E18" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F18">
-        <v>8.8663036902600897E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8.8663037E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" t="s">
         <v>34</v>
       </c>
-      <c r="D19" t="s">
-        <v>18</v>
-      </c>
       <c r="E19" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F19">
-        <v>4.5952813067150503E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+        <v>4.5952813000000002E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="E20" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F20">
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="E21" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F21">
         <v>0.20100000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="E22" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F22">
         <v>0.23</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D23" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E23" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F23">
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="E24" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F24">
         <v>0.1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="E25" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F25">
         <v>1.24</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="E26" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F26">
         <v>3.2650000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C27" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="E27" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F27">
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E28" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F28">
         <v>1.8109999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E29" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F29">
         <v>3.4129999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D30" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="E30" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F30">
         <v>18.690000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" t="s">
+        <v>44</v>
+      </c>
+      <c r="G31" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" t="s">
+        <v>46</v>
+      </c>
+      <c r="G32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" t="s">
         <v>29</v>
       </c>
-      <c r="D31" t="s">
-        <v>37</v>
-      </c>
-      <c r="E31" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="F33">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" t="s">
         <v>29</v>
       </c>
-      <c r="D32" t="s">
-        <v>39</v>
-      </c>
-      <c r="E32" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>41</v>
-      </c>
-      <c r="B33" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33" t="s">
-        <v>28</v>
-      </c>
-      <c r="D33" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>41</v>
-      </c>
-      <c r="B34" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34" t="s">
-        <v>28</v>
-      </c>
-      <c r="D34" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F34">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C35" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D35" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+      <c r="E35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F35">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C36" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D36" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="E36" t="s">
+        <v>29</v>
+      </c>
+      <c r="F36">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C37" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D37" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+      <c r="E37" t="s">
+        <v>29</v>
+      </c>
+      <c r="F37">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C38" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D38" t="s">
-        <v>47</v>
+        <v>55</v>
+      </c>
+      <c r="E38" t="s">
+        <v>29</v>
+      </c>
+      <c r="F38">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" t="s">
+        <v>57</v>
+      </c>
+      <c r="G39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008ECAB31773B3D64A955B79DCECF3D75D" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2078a7c437835ce6ccc54ed572140080">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1812b7d3-e7a1-454a-96a7-d89f9c45d61a" xmlns:ns3="6a4f18d6-d02c-47de-8192-877c1ae6ba95" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b5cdadb961a881ff75adc1ded15049d8" ns2:_="" ns3:_="">
-    <xsd:import namespace="1812b7d3-e7a1-454a-96a7-d89f9c45d61a"/>
-    <xsd:import namespace="6a4f18d6-d02c-47de-8192-877c1ae6ba95"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="1812b7d3-e7a1-454a-96a7-d89f9c45d61a" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="11" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="12" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="13" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="17" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="18" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="6a4f18d6-d02c-47de-8192-877c1ae6ba95" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="14" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="15" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9C5F6C2-448D-41A5-85E3-FC5B0984219A}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD0D86AA-7393-44A9-8AF0-C18803440492}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FC63F5E-9223-4420-9E31-1ED9C5BAC8D5}"/>
 </file>
</xml_diff>

<commit_message>
Adding salty zoop species
</commit_message>
<xml_diff>
--- a/data/data_in/Zoop Categories for SEM.xlsx
+++ b/data/data_in/Zoop Categories for SEM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\swg-21-foodwebs\data\data_in\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\NCEAS Working Group\Food Web Group\swg-21-foodwebs\data\data_in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD334AB-B89B-4070-9F88-7705C8CA8356}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F3EADF-EEF6-4410-A0F7-1C93CE9C063A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zoop Categories for SEM" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="67">
   <si>
     <t>SEM Category</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Predatory copepods have predatory nauplii?</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Calanoid Copepod</t>
   </si>
   <si>
@@ -221,6 +218,18 @@
   </si>
   <si>
     <t>Hyalella spp</t>
+  </si>
+  <si>
+    <t>Salinity Range</t>
+  </si>
+  <si>
+    <t>Marine</t>
+  </si>
+  <si>
+    <t>LSZ</t>
+  </si>
+  <si>
+    <t>Fresh</t>
   </si>
 </sst>
 </file>
@@ -1061,22 +1070,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.76171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.9375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.29296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.41015625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.9375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.453125" customWidth="1"/>
+    <col min="2" max="2" width="20.54296875" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.26953125" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1098,8 +1110,11 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1122,15 +1137,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
         <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -1138,36 +1156,45 @@
       <c r="F3">
         <v>1.3009999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
       </c>
       <c r="F4">
         <v>2.984</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -1175,133 +1202,151 @@
       <c r="F5">
         <v>1.1619999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6">
         <v>2.6659999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
         <v>21</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" t="s">
-        <v>22</v>
       </c>
       <c r="F8">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F11">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -1309,124 +1354,151 @@
       <c r="F12">
         <v>1.4430000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F13">
         <v>3.55</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
         <v>27</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>28</v>
-      </c>
-      <c r="E14" t="s">
-        <v>29</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
         <v>30</v>
       </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" t="s">
-        <v>31</v>
-      </c>
       <c r="E15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F15">
         <v>3.36</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F16">
         <v>0.13300000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F17">
         <v>0.13300000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F18">
         <v>8.8663037E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1434,19 +1506,22 @@
       <c r="F19">
         <v>4.5952813000000002E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
         <v>16</v>
       </c>
-      <c r="B20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" t="s">
-        <v>17</v>
-      </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1455,98 +1530,101 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
         <v>16</v>
       </c>
-      <c r="B21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" t="s">
-        <v>17</v>
-      </c>
       <c r="D21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F21">
         <v>0.20100000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
         <v>16</v>
       </c>
-      <c r="B22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" t="s">
-        <v>17</v>
-      </c>
       <c r="D22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F22">
         <v>0.23</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s">
         <v>16</v>
       </c>
-      <c r="B23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" t="s">
-        <v>17</v>
-      </c>
       <c r="D23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F23">
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F24">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
@@ -1554,59 +1632,68 @@
       <c r="F25">
         <v>1.24</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C26" t="s">
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F26">
         <v>3.2650000000000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C27" t="s">
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F27">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C28" t="s">
         <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -1614,286 +1701,301 @@
       <c r="F28">
         <v>1.8109999999999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C29" t="s">
         <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F29">
         <v>3.4129999999999998</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" t="s">
         <v>16</v>
       </c>
-      <c r="B30" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" t="s">
-        <v>17</v>
-      </c>
       <c r="D30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F30">
         <v>18.690000000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" t="s">
         <v>43</v>
       </c>
-      <c r="B31" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" t="s">
-        <v>17</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="G31" t="s">
         <v>44</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A32" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="G32" t="s">
         <v>46</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A33" t="s">
+      <c r="B33" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" t="s">
         <v>48</v>
       </c>
-      <c r="B33" t="s">
-        <v>48</v>
-      </c>
-      <c r="C33" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" t="s">
-        <v>49</v>
-      </c>
       <c r="E33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F33">
         <v>0.04</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C34" t="s">
         <v>9</v>
       </c>
       <c r="D34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F34">
         <v>0.12</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F35">
         <v>0.3</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C36" t="s">
+        <v>51</v>
+      </c>
+      <c r="D36" t="s">
         <v>52</v>
       </c>
-      <c r="D36" t="s">
-        <v>53</v>
-      </c>
       <c r="E36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F36">
         <v>0.12</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C37" t="s">
         <v>9</v>
       </c>
       <c r="D37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F37">
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C38" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E38" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F38">
         <v>0.12</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" t="s">
         <v>56</v>
       </c>
-      <c r="B39" t="s">
-        <v>56</v>
-      </c>
-      <c r="C39" t="s">
-        <v>9</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="G39" t="s">
         <v>57</v>
       </c>
-      <c r="G39" t="s">
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A40" t="s">
-        <v>56</v>
-      </c>
-      <c r="B40" t="s">
-        <v>56</v>
-      </c>
-      <c r="C40" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A41" t="s">
-        <v>56</v>
-      </c>
-      <c r="B41" t="s">
-        <v>56</v>
-      </c>
-      <c r="C41" t="s">
-        <v>9</v>
-      </c>
-      <c r="D41" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A42" t="s">
-        <v>56</v>
-      </c>
-      <c r="B42" t="s">
-        <v>56</v>
-      </c>
-      <c r="C42" t="s">
-        <v>9</v>
-      </c>
-      <c r="D42" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A43" t="s">
-        <v>56</v>
-      </c>
-      <c r="B43" t="s">
-        <v>56</v>
-      </c>
-      <c r="C43" t="s">
-        <v>9</v>
-      </c>
-      <c r="D43" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A44" t="s">
-        <v>56</v>
-      </c>
-      <c r="B44" t="s">
-        <v>56</v>
-      </c>
-      <c r="C44" t="s">
-        <v>9</v>
-      </c>
-      <c r="D44" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update biomass values, add missing lifestages and zoop categories for SEM
</commit_message>
<xml_diff>
--- a/data/data_in/Zoop Categories for SEM.xlsx
+++ b/data/data_in/Zoop Categories for SEM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\NCEAS Working Group\Food Web Group\swg-21-foodwebs\data\data_in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F3EADF-EEF6-4410-A0F7-1C93CE9C063A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6985956F-17A2-4A5B-814B-348A42222538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="15930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zoop Categories for SEM" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="69">
   <si>
     <t>SEM Category</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Juvenile</t>
   </si>
   <si>
-    <t>Predatory copepods have predatory nauplii?</t>
-  </si>
-  <si>
     <t>Calanoid Copepod</t>
   </si>
   <si>
@@ -133,18 +130,12 @@
     <t>Limnoithona tetraspina</t>
   </si>
   <si>
-    <t>Oithona</t>
-  </si>
-  <si>
     <t>Oithona davisae</t>
   </si>
   <si>
     <t>Oithona similis</t>
   </si>
   <si>
-    <t>Pseudodiaptomus</t>
-  </si>
-  <si>
     <t>Pseudodiaptomus forbesi</t>
   </si>
   <si>
@@ -193,9 +184,6 @@
     <t>Polyarthra</t>
   </si>
   <si>
-    <t>Other Rotifer</t>
-  </si>
-  <si>
     <t>Amphipods</t>
   </si>
   <si>
@@ -230,13 +218,31 @@
   </si>
   <si>
     <t>Fresh</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Excluded b/c of multiple feeding strategies</t>
+  </si>
+  <si>
+    <t>High Salinity</t>
+  </si>
+  <si>
+    <t>Oithona spp.</t>
+  </si>
+  <si>
+    <t>Pseudodiaptomus spp.</t>
+  </si>
+  <si>
+    <t>Tortanus spp.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -371,6 +377,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -553,7 +572,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -668,8 +687,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -712,11 +755,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
@@ -754,6 +805,7 @@
     <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal_CB BPUE Calculation" xfId="42" xr:uid="{EC2A37EB-BACF-4500-B750-9CDA6323C6C1}"/>
     <cellStyle name="Note" xfId="37" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="38" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="39" builtinId="15" customBuiltin="1"/>
@@ -1070,10 +1122,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1089,141 +1141,141 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>63</v>
+      <c r="H1" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F2">
-        <v>0.1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
+        <v>0.6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F3">
-        <v>1.3009999999999999</v>
+        <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4">
-        <v>2.984</v>
+        <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F5">
-        <v>1.1619999999999999</v>
+        <v>2.984</v>
       </c>
       <c r="H5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F6">
-        <v>2.6659999999999999</v>
+        <v>1.3009999999999999</v>
       </c>
       <c r="H6" t="s">
         <v>65</v>
@@ -1231,10 +1283,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -1243,13 +1295,13 @@
         <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F7">
-        <v>0.6</v>
+        <v>3.8</v>
       </c>
       <c r="H7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -1257,65 +1309,65 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F8">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="H8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>4</v>
-      </c>
-      <c r="H9" t="s">
-        <v>66</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>3.55</v>
+      </c>
+      <c r="H10" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -1323,16 +1375,22 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
       </c>
       <c r="D11" t="s">
         <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F11">
-        <v>4</v>
+        <v>1.4430000000000001</v>
+      </c>
+      <c r="H11" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -1340,22 +1398,22 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F12">
-        <v>1.4430000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="H12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -1363,22 +1421,16 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="F13">
-        <v>3.55</v>
-      </c>
-      <c r="H13" t="s">
-        <v>65</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -1386,36 +1438,45 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="H14" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s">
         <v>30</v>
       </c>
       <c r="E15" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F15">
-        <v>3.36</v>
+        <v>0.04</v>
+      </c>
+      <c r="H15" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -1423,7 +1484,7 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
@@ -1432,13 +1493,13 @@
         <v>31</v>
       </c>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F16">
         <v>0.13300000000000001</v>
       </c>
       <c r="H16" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -1446,22 +1507,22 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E17" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F17">
-        <v>0.13300000000000001</v>
+        <v>0.04</v>
       </c>
       <c r="H17" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -1469,22 +1530,22 @@
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F18">
         <v>8.8663037E-2</v>
       </c>
       <c r="H18" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1492,13 +1553,13 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1507,87 +1568,99 @@
         <v>4.5952813000000002E-2</v>
       </c>
       <c r="H19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20">
-        <v>6.6000000000000003E-2</v>
+        <v>13</v>
+      </c>
+      <c r="F20" s="3">
+        <v>3.2650000000000001</v>
+      </c>
+      <c r="H20" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E21" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F21">
-        <v>0.20100000000000001</v>
+        <v>1.24</v>
+      </c>
+      <c r="H21" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F22">
-        <v>0.23</v>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="H22" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="E23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F23">
-        <v>0.57999999999999996</v>
+        <v>0.1</v>
+      </c>
+      <c r="H23" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -1595,22 +1668,22 @@
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="E24" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F24">
-        <v>0.1</v>
+        <v>1.252</v>
       </c>
       <c r="H24" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -1618,22 +1691,22 @@
         <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="E25" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F25">
-        <v>1.24</v>
+        <v>0.1</v>
       </c>
       <c r="H25" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
@@ -1641,22 +1714,22 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C26" t="s">
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F26">
-        <v>3.2650000000000001</v>
+        <v>3.4129999999999998</v>
       </c>
       <c r="H26" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -1664,22 +1737,22 @@
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C27" t="s">
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E27" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F27">
-        <v>4.9000000000000004</v>
+        <v>1.8109999999999999</v>
       </c>
       <c r="H27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -1687,318 +1760,492 @@
         <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C28" t="s">
         <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E28" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F28">
-        <v>1.8109999999999999</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H28" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="C29" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D29" t="s">
-        <v>40</v>
-      </c>
-      <c r="E29" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29">
-        <v>3.4129999999999998</v>
+        <v>42</v>
+      </c>
+      <c r="G29" t="s">
+        <v>43</v>
       </c>
       <c r="H29" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" t="s">
         <v>15</v>
       </c>
-      <c r="B30" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" t="s">
-        <v>16</v>
-      </c>
       <c r="D30" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" t="s">
         <v>41</v>
       </c>
-      <c r="E30" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30">
-        <v>18.690000000000001</v>
-      </c>
       <c r="H30" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D31" t="s">
-        <v>43</v>
+        <v>8</v>
+      </c>
+      <c r="E31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31">
+        <v>0.1</v>
       </c>
       <c r="G31" t="s">
-        <v>44</v>
-      </c>
-      <c r="H31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32">
+        <v>3.36</v>
+      </c>
+      <c r="H32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" t="s">
         <v>16</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E33" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33">
+        <v>2.6659999999999999</v>
+      </c>
+      <c r="H33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34">
+        <v>1.1619999999999999</v>
+      </c>
+      <c r="H34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35">
+        <v>0.23</v>
+      </c>
+      <c r="H35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" t="s">
+        <v>34</v>
+      </c>
+      <c r="E36" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="H36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" t="s">
+        <v>66</v>
+      </c>
+      <c r="E37" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="H37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" t="s">
+        <v>66</v>
+      </c>
+      <c r="E38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="4">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="H38" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="3">
+        <v>18.690000000000001</v>
+      </c>
+      <c r="H39" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" t="s">
+        <v>68</v>
+      </c>
+      <c r="E40" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="1">
+        <v>7.9480000000000004</v>
+      </c>
+      <c r="H40" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" t="s">
+        <v>47</v>
+      </c>
+      <c r="E41" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" t="s">
         <v>45</v>
       </c>
-      <c r="G32" t="s">
+      <c r="E42" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42">
+        <v>0.04</v>
+      </c>
+      <c r="H42" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" t="s">
+        <v>50</v>
+      </c>
+      <c r="E43" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" t="s">
         <v>46</v>
       </c>
-      <c r="H32" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33" t="s">
-        <v>47</v>
-      </c>
-      <c r="C33" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="E44" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" t="s">
         <v>48</v>
       </c>
-      <c r="E33" t="s">
-        <v>28</v>
-      </c>
-      <c r="F33">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>47</v>
-      </c>
-      <c r="B34" t="s">
-        <v>47</v>
-      </c>
-      <c r="C34" t="s">
-        <v>9</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="D45" t="s">
         <v>49</v>
       </c>
-      <c r="E34" t="s">
-        <v>28</v>
-      </c>
-      <c r="F34">
+      <c r="E45" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45">
         <v>0.12</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>47</v>
-      </c>
-      <c r="B35" t="s">
-        <v>47</v>
-      </c>
-      <c r="C35" t="s">
-        <v>16</v>
-      </c>
-      <c r="D35" t="s">
-        <v>50</v>
-      </c>
-      <c r="E35" t="s">
-        <v>28</v>
-      </c>
-      <c r="F35">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>47</v>
-      </c>
-      <c r="B36" t="s">
-        <v>47</v>
-      </c>
-      <c r="C36" t="s">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>51</v>
       </c>
-      <c r="D36" t="s">
+      <c r="B46" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" t="s">
         <v>52</v>
       </c>
-      <c r="E36" t="s">
-        <v>28</v>
-      </c>
-      <c r="F36">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>47</v>
-      </c>
-      <c r="B37" t="s">
-        <v>47</v>
-      </c>
-      <c r="C37" t="s">
-        <v>9</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="G50" t="s">
         <v>53</v>
       </c>
-      <c r="E37" t="s">
-        <v>28</v>
-      </c>
-      <c r="F37">
-        <v>0.28000000000000003</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>47</v>
-      </c>
-      <c r="B38" t="s">
-        <v>47</v>
-      </c>
-      <c r="C38" t="s">
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>51</v>
       </c>
-      <c r="D38" t="s">
-        <v>54</v>
-      </c>
-      <c r="E38" t="s">
-        <v>28</v>
-      </c>
-      <c r="F38">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>55</v>
-      </c>
-      <c r="B39" t="s">
-        <v>55</v>
-      </c>
-      <c r="C39" t="s">
-        <v>9</v>
-      </c>
-      <c r="D39" t="s">
-        <v>56</v>
-      </c>
-      <c r="G39" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>55</v>
-      </c>
-      <c r="B40" t="s">
-        <v>55</v>
-      </c>
-      <c r="C40" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="B51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>55</v>
-      </c>
-      <c r="B41" t="s">
-        <v>55</v>
-      </c>
-      <c r="C41" t="s">
-        <v>9</v>
-      </c>
-      <c r="D41" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>55</v>
-      </c>
-      <c r="B42" t="s">
-        <v>55</v>
-      </c>
-      <c r="C42" t="s">
-        <v>9</v>
-      </c>
-      <c r="D42" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>55</v>
-      </c>
-      <c r="B43" t="s">
-        <v>55</v>
-      </c>
-      <c r="C43" t="s">
-        <v>9</v>
-      </c>
-      <c r="D43" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>55</v>
-      </c>
-      <c r="B44" t="s">
-        <v>55</v>
-      </c>
-      <c r="C44" t="s">
-        <v>9</v>
-      </c>
-      <c r="D44" t="s">
-        <v>62</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H49">
+    <sortCondition ref="A2:A49"/>
+    <sortCondition ref="D2:D49"/>
+    <sortCondition ref="E2:E49"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add missing categories, change which are counted in meso or micro net, and filtered out copepod nauplii as a group
</commit_message>
<xml_diff>
--- a/data/data_in/Zoop Categories for SEM.xlsx
+++ b/data/data_in/Zoop Categories for SEM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\NCEAS Working Group\Food Web Group\swg-21-foodwebs\data\data_in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6985956F-17A2-4A5B-814B-348A42222538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E62C02-EE50-4C8E-B140-FF6D1A161E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="15930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zoop Categories for SEM" sheetId="1" r:id="rId1"/>
@@ -166,76 +166,76 @@
     <t>Rotifers</t>
   </si>
   <si>
+    <t>Omnivorous</t>
+  </si>
+  <si>
+    <t>Amphipods</t>
+  </si>
+  <si>
+    <t>Gammarus daiberi</t>
+  </si>
+  <si>
+    <t>Use EMP benthic for amphipods, only CPUE</t>
+  </si>
+  <si>
+    <t>Americorophium spinicorne</t>
+  </si>
+  <si>
+    <t>Americorophium stimpsoni</t>
+  </si>
+  <si>
+    <t>Ampelisca abdita</t>
+  </si>
+  <si>
+    <t>Corophium alienense</t>
+  </si>
+  <si>
+    <t>Hyalella spp</t>
+  </si>
+  <si>
+    <t>Salinity Range</t>
+  </si>
+  <si>
+    <t>Marine</t>
+  </si>
+  <si>
+    <t>LSZ</t>
+  </si>
+  <si>
+    <t>Fresh</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Excluded b/c of multiple feeding strategies</t>
+  </si>
+  <si>
+    <t>High Salinity</t>
+  </si>
+  <si>
+    <t>Oithona spp.</t>
+  </si>
+  <si>
+    <t>Pseudodiaptomus spp.</t>
+  </si>
+  <si>
+    <t>Tortanus spp.</t>
+  </si>
+  <si>
     <t>Keratella</t>
   </si>
   <si>
+    <t>Asplanchna</t>
+  </si>
+  <si>
     <t>Synchaeta</t>
   </si>
   <si>
-    <t>Asplanchna</t>
-  </si>
-  <si>
-    <t>Omnivorous</t>
-  </si>
-  <si>
     <t>Trichocerca</t>
   </si>
   <si>
     <t>Polyarthra</t>
-  </si>
-  <si>
-    <t>Amphipods</t>
-  </si>
-  <si>
-    <t>Gammarus daiberi</t>
-  </si>
-  <si>
-    <t>Use EMP benthic for amphipods, only CPUE</t>
-  </si>
-  <si>
-    <t>Americorophium spinicorne</t>
-  </si>
-  <si>
-    <t>Americorophium stimpsoni</t>
-  </si>
-  <si>
-    <t>Ampelisca abdita</t>
-  </si>
-  <si>
-    <t>Corophium alienense</t>
-  </si>
-  <si>
-    <t>Hyalella spp</t>
-  </si>
-  <si>
-    <t>Salinity Range</t>
-  </si>
-  <si>
-    <t>Marine</t>
-  </si>
-  <si>
-    <t>LSZ</t>
-  </si>
-  <si>
-    <t>Fresh</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Excluded b/c of multiple feeding strategies</t>
-  </si>
-  <si>
-    <t>High Salinity</t>
-  </si>
-  <si>
-    <t>Oithona spp.</t>
-  </si>
-  <si>
-    <t>Pseudodiaptomus spp.</t>
-  </si>
-  <si>
-    <t>Tortanus spp.</t>
   </si>
 </sst>
 </file>
@@ -1125,7 +1125,7 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1163,7 +1163,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -1186,7 +1186,7 @@
         <v>0.6</v>
       </c>
       <c r="H2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -1209,7 +1209,7 @@
         <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -1232,7 +1232,7 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -1255,7 +1255,7 @@
         <v>2.984</v>
       </c>
       <c r="H5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -1278,7 +1278,7 @@
         <v>1.3009999999999999</v>
       </c>
       <c r="H6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -1301,7 +1301,7 @@
         <v>3.8</v>
       </c>
       <c r="H7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -1324,7 +1324,7 @@
         <v>4</v>
       </c>
       <c r="H8" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -1367,7 +1367,7 @@
         <v>3.55</v>
       </c>
       <c r="H10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -1390,7 +1390,7 @@
         <v>1.4430000000000001</v>
       </c>
       <c r="H11" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -1413,7 +1413,7 @@
         <v>0.1</v>
       </c>
       <c r="H12" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -1453,7 +1453,7 @@
         <v>0.13300000000000001</v>
       </c>
       <c r="H14" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -1476,7 +1476,7 @@
         <v>0.04</v>
       </c>
       <c r="H15" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -1499,7 +1499,7 @@
         <v>0.13300000000000001</v>
       </c>
       <c r="H16" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -1522,7 +1522,7 @@
         <v>0.04</v>
       </c>
       <c r="H17" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -1545,7 +1545,7 @@
         <v>8.8663037E-2</v>
       </c>
       <c r="H18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1568,7 +1568,7 @@
         <v>4.5952813000000002E-2</v>
       </c>
       <c r="H19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -1591,7 +1591,7 @@
         <v>3.2650000000000001</v>
       </c>
       <c r="H20" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -1614,7 +1614,7 @@
         <v>1.24</v>
       </c>
       <c r="H21" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -1637,7 +1637,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="H22" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -1651,7 +1651,7 @@
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E23" t="s">
         <v>13</v>
@@ -1660,7 +1660,7 @@
         <v>0.1</v>
       </c>
       <c r="H23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -1674,7 +1674,7 @@
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1683,7 +1683,7 @@
         <v>1.252</v>
       </c>
       <c r="H24" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -1697,7 +1697,7 @@
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E25" t="s">
         <v>20</v>
@@ -1706,7 +1706,7 @@
         <v>0.1</v>
       </c>
       <c r="H25" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
@@ -1729,7 +1729,7 @@
         <v>3.4129999999999998</v>
       </c>
       <c r="H26" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -1752,7 +1752,7 @@
         <v>1.8109999999999999</v>
       </c>
       <c r="H27" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -1775,7 +1775,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H28" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
@@ -1795,7 +1795,7 @@
         <v>43</v>
       </c>
       <c r="H29" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -1816,12 +1816,12 @@
         <v>41</v>
       </c>
       <c r="H30" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
@@ -1839,7 +1839,7 @@
         <v>0.1</v>
       </c>
       <c r="G31" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -1862,7 +1862,7 @@
         <v>3.36</v>
       </c>
       <c r="H32" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
@@ -1885,7 +1885,7 @@
         <v>2.6659999999999999</v>
       </c>
       <c r="H33" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
@@ -1908,7 +1908,7 @@
         <v>1.1619999999999999</v>
       </c>
       <c r="H34" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -1931,7 +1931,7 @@
         <v>0.23</v>
       </c>
       <c r="H35" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
@@ -1954,7 +1954,7 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="H36" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
@@ -1968,7 +1968,7 @@
         <v>15</v>
       </c>
       <c r="D37" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E37" t="s">
         <v>13</v>
@@ -1977,7 +1977,7 @@
         <v>0.20100000000000001</v>
       </c>
       <c r="H37" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
@@ -1991,7 +1991,7 @@
         <v>15</v>
       </c>
       <c r="D38" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E38" t="s">
         <v>10</v>
@@ -2000,7 +2000,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="H38" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
@@ -2023,7 +2023,7 @@
         <v>18.690000000000001</v>
       </c>
       <c r="H39" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
@@ -2037,7 +2037,7 @@
         <v>15</v>
       </c>
       <c r="D40" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E40" t="s">
         <v>10</v>
@@ -2046,7 +2046,7 @@
         <v>7.9480000000000004</v>
       </c>
       <c r="H40" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
@@ -2060,7 +2060,7 @@
         <v>15</v>
       </c>
       <c r="D41" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="E41" t="s">
         <v>13</v>
@@ -2080,7 +2080,7 @@
         <v>9</v>
       </c>
       <c r="D42" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="E42" t="s">
         <v>13</v>
@@ -2089,7 +2089,7 @@
         <v>0.04</v>
       </c>
       <c r="H42" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
@@ -2103,7 +2103,7 @@
         <v>9</v>
       </c>
       <c r="D43" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="E43" t="s">
         <v>13</v>
@@ -2123,7 +2123,7 @@
         <v>9</v>
       </c>
       <c r="D44" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="E44" t="s">
         <v>13</v>
@@ -2140,10 +2140,10 @@
         <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D45" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="E45" t="s">
         <v>13</v>
@@ -2154,89 +2154,89 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C46" t="s">
         <v>9</v>
       </c>
       <c r="D46" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C47" t="s">
         <v>9</v>
       </c>
       <c r="D47" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" t="s">
         <v>51</v>
-      </c>
-      <c r="B48" t="s">
-        <v>51</v>
-      </c>
-      <c r="C48" t="s">
-        <v>9</v>
-      </c>
-      <c r="D48" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C49" t="s">
         <v>9</v>
       </c>
       <c r="D49" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B50" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C50" t="s">
         <v>9</v>
       </c>
       <c r="D50" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G50" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B51" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C51" t="s">
         <v>9</v>
       </c>
       <c r="D51" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update zoop biomass conversions and added rotifers to SEM category file
</commit_message>
<xml_diff>
--- a/data/data_in/Zoop Categories for SEM.xlsx
+++ b/data/data_in/Zoop Categories for SEM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\swg-21-foodwebs\data\data_in\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\NCEAS Working Group\Food Web Group\swg-21-foodwebs\data\data_in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186C6438-5D40-4F96-BD64-10C1BB2FE2B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF49607-9317-4D0D-B8CA-DAF0E8B2EE75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zoop Categories for SEM" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="68">
   <si>
     <t>SEM Category</t>
   </si>
@@ -202,9 +202,6 @@
     <t>Fresh</t>
   </si>
   <si>
-    <t>Excluded b/c of multiple feeding strategies</t>
-  </si>
-  <si>
     <t>High Salinity</t>
   </si>
   <si>
@@ -233,6 +230,9 @@
   </si>
   <si>
     <t>Pseudodiaptomus</t>
+  </si>
+  <si>
+    <t>Pseudodiaptomus spp.</t>
   </si>
 </sst>
 </file>
@@ -569,7 +569,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -685,21 +685,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -754,15 +739,17 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1119,51 +1106,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.46875" customWidth="1"/>
-    <col min="2" max="2" width="20.52734375" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.3515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.87890625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.29296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.29296875" customWidth="1"/>
-    <col min="8" max="8" width="12.29296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1173,20 +1160,20 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>0.6</v>
       </c>
       <c r="H2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1196,20 +1183,20 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>4</v>
       </c>
       <c r="H3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1219,20 +1206,20 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>1</v>
       </c>
       <c r="H4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1242,20 +1229,20 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
       </c>
-      <c r="F5">
-        <v>2.984</v>
+      <c r="F5" s="3">
+        <v>2.98</v>
       </c>
       <c r="H5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1265,43 +1252,43 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
       </c>
-      <c r="F6">
-        <v>1.3009999999999999</v>
+      <c r="F6" s="3">
+        <v>1.3</v>
       </c>
       <c r="H6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" t="s">
-        <v>19</v>
+      <c r="D7" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7">
-        <v>3.8</v>
+        <v>13</v>
+      </c>
+      <c r="F7" s="3">
+        <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1311,20 +1298,20 @@
       <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="F8" s="3">
+        <v>2</v>
       </c>
       <c r="H8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1334,17 +1321,20 @@
       <c r="C9" t="s">
         <v>9</v>
       </c>
-      <c r="D9" t="s">
-        <v>23</v>
+      <c r="D9" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
+        <v>13</v>
+      </c>
+      <c r="F9" s="3">
+        <v>3.55</v>
+      </c>
+      <c r="H9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1354,20 +1344,20 @@
       <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10">
-        <v>3.55</v>
+        <v>10</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1.4430000000000001</v>
       </c>
       <c r="H10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1377,20 +1367,20 @@
       <c r="C11" t="s">
         <v>9</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11">
-        <v>1.4430000000000001</v>
+        <v>20</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.1</v>
       </c>
       <c r="H11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1400,515 +1390,519 @@
       <c r="C12" t="s">
         <v>9</v>
       </c>
-      <c r="D12" t="s">
-        <v>24</v>
+      <c r="D12" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="E12" t="s">
         <v>20</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="3">
         <v>0.1</v>
       </c>
       <c r="H12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" t="s">
-        <v>26</v>
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.5">
+        <v>13</v>
+      </c>
+      <c r="F13" s="4">
+        <v>2.66</v>
+      </c>
+      <c r="H13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
       </c>
-      <c r="D14" t="s">
-        <v>30</v>
+      <c r="D14" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="E14" t="s">
         <v>13</v>
       </c>
-      <c r="F14">
-        <v>0.13300000000000001</v>
+      <c r="F14" s="3">
+        <v>4.9000000000000004</v>
       </c>
       <c r="H14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
-      <c r="D15" t="s">
-        <v>30</v>
+      <c r="D15" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
       </c>
-      <c r="F15">
-        <v>0.04</v>
+      <c r="F15" s="3">
+        <v>1.1499999999999999</v>
       </c>
       <c r="H15" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
       </c>
-      <c r="D16" t="s">
-        <v>31</v>
+      <c r="D16" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="E16" t="s">
         <v>13</v>
       </c>
-      <c r="F16">
-        <v>0.13300000000000001</v>
+      <c r="F16" s="3">
+        <v>3.4129999999999998</v>
       </c>
       <c r="H16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
       </c>
-      <c r="D17" t="s">
-        <v>31</v>
+      <c r="D17" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
       </c>
-      <c r="F17">
-        <v>0.04</v>
+      <c r="F17" s="3">
+        <v>1.8109999999999999</v>
       </c>
       <c r="H17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
       </c>
-      <c r="D18" t="s">
-        <v>32</v>
+      <c r="D18" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="E18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18">
-        <v>8.8663037E-2</v>
+        <v>20</v>
+      </c>
+      <c r="F18" s="3">
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
       </c>
-      <c r="D19" t="s">
-        <v>32</v>
+      <c r="D19" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="E19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19">
-        <v>4.5952813000000002E-2</v>
+        <v>20</v>
+      </c>
+      <c r="F19" s="3">
+        <v>3.8</v>
       </c>
       <c r="H19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
       </c>
-      <c r="D20" t="s">
-        <v>35</v>
+      <c r="D20" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="E20" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F20" s="3">
-        <v>3.2650000000000001</v>
-      </c>
-      <c r="H20" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
       </c>
-      <c r="D21" t="s">
-        <v>35</v>
+      <c r="D21" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="E21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21">
-        <v>1.24</v>
+        <v>13</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0.13300000000000001</v>
       </c>
       <c r="H21" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
       </c>
-      <c r="D22" t="s">
-        <v>36</v>
+      <c r="D22" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="E22" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22">
-        <v>4.9000000000000004</v>
+        <v>10</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0.04</v>
       </c>
       <c r="H22" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
       </c>
-      <c r="D23" t="s">
-        <v>67</v>
+      <c r="D23" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="E23" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23">
-        <v>0.1</v>
+        <v>20</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0.02</v>
       </c>
       <c r="H23" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
       </c>
-      <c r="D24" t="s">
-        <v>67</v>
+      <c r="D24" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="E24" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24">
-        <v>1.252</v>
+        <v>13</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0.13300000000000001</v>
       </c>
       <c r="H24" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
       </c>
-      <c r="D25" t="s">
-        <v>67</v>
+      <c r="D25" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="E25" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25">
-        <v>0.1</v>
+        <v>13</v>
+      </c>
+      <c r="F25" s="3">
+        <v>8.8663037E-2</v>
       </c>
       <c r="H25" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
       <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" t="s">
+        <v>43</v>
+      </c>
+      <c r="H27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="5"/>
+      <c r="G28" t="s">
+        <v>41</v>
+      </c>
+      <c r="H28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" t="s">
         <v>11</v>
-      </c>
-      <c r="C26" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26">
-        <v>3.4129999999999998</v>
-      </c>
-      <c r="H26" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27">
-        <v>1.8109999999999999</v>
-      </c>
-      <c r="H27" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A28" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28" t="s">
-        <v>37</v>
-      </c>
-      <c r="E28" t="s">
-        <v>20</v>
-      </c>
-      <c r="F28">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="H28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="B29" t="s">
-        <v>39</v>
       </c>
       <c r="C29" t="s">
         <v>15</v>
       </c>
-      <c r="D29" t="s">
-        <v>42</v>
+      <c r="D29" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="E29" t="s">
         <v>13</v>
       </c>
-      <c r="G29" t="s">
-        <v>43</v>
+      <c r="F29" s="3">
+        <v>2.6659999999999999</v>
       </c>
       <c r="H29" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
       <c r="B30" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="C30" t="s">
         <v>15</v>
       </c>
-      <c r="D30" t="s">
-        <v>40</v>
+      <c r="D30" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="E30" t="s">
-        <v>13</v>
-      </c>
-      <c r="F30" s="2"/>
-      <c r="G30" t="s">
-        <v>41</v>
+        <v>10</v>
+      </c>
+      <c r="F30" s="3">
+        <v>1.1619999999999999</v>
       </c>
       <c r="H30" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C31" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" t="s">
-        <v>64</v>
+        <v>15</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="E31" t="s">
-        <v>20</v>
-      </c>
-      <c r="F31">
-        <v>0.1</v>
-      </c>
-      <c r="G31" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="4">
+        <v>15.89</v>
+      </c>
+      <c r="H31" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>14</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C32" t="s">
         <v>15</v>
       </c>
-      <c r="D32" t="s">
-        <v>29</v>
+      <c r="D32" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="E32" t="s">
-        <v>13</v>
-      </c>
-      <c r="F32">
-        <v>3.36</v>
+        <v>10</v>
+      </c>
+      <c r="F32" s="6">
+        <v>7.9480000000000004</v>
       </c>
       <c r="H32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>14</v>
       </c>
       <c r="B33" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C33" t="s">
         <v>15</v>
       </c>
-      <c r="D33" t="s">
-        <v>16</v>
+      <c r="D33" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="E33" t="s">
         <v>13</v>
       </c>
-      <c r="F33">
-        <v>2.6659999999999999</v>
+      <c r="F33" s="3">
+        <v>3.36</v>
       </c>
       <c r="H33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>14</v>
       </c>
       <c r="B34" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C34" t="s">
         <v>15</v>
       </c>
-      <c r="D34" t="s">
-        <v>16</v>
+      <c r="D34" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="E34" t="s">
-        <v>10</v>
-      </c>
-      <c r="F34">
-        <v>1.1619999999999999</v>
+        <v>13</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0.20100000000000001</v>
       </c>
       <c r="H34" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -1918,20 +1912,20 @@
       <c r="C35" t="s">
         <v>15</v>
       </c>
-      <c r="D35" t="s">
-        <v>33</v>
+      <c r="D35" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="E35" t="s">
-        <v>13</v>
-      </c>
-      <c r="F35">
-        <v>0.23</v>
+        <v>10</v>
+      </c>
+      <c r="F35" s="5">
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="H35" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -1941,20 +1935,20 @@
       <c r="C36" t="s">
         <v>15</v>
       </c>
-      <c r="D36" t="s">
-        <v>34</v>
+      <c r="D36" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="E36" t="s">
         <v>13</v>
       </c>
-      <c r="F36">
-        <v>0.57999999999999996</v>
+      <c r="F36" s="3">
+        <v>0.21</v>
       </c>
       <c r="H36" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -1964,89 +1958,83 @@
       <c r="C37" t="s">
         <v>15</v>
       </c>
-      <c r="D37" t="s">
-        <v>66</v>
+      <c r="D37" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="E37" t="s">
         <v>13</v>
       </c>
-      <c r="F37">
-        <v>0.20100000000000001</v>
+      <c r="F37" s="3">
+        <v>0.5</v>
       </c>
       <c r="H37" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C38" t="s">
         <v>15</v>
       </c>
-      <c r="D38" t="s">
-        <v>66</v>
+      <c r="D38" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="E38" t="s">
-        <v>10</v>
-      </c>
-      <c r="F38" s="4">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="H38" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A39" t="s">
-        <v>14</v>
-      </c>
-      <c r="B39" t="s">
-        <v>11</v>
-      </c>
-      <c r="C39" t="s">
-        <v>15</v>
-      </c>
-      <c r="D39" t="s">
-        <v>38</v>
-      </c>
       <c r="E39" t="s">
         <v>13</v>
       </c>
       <c r="F39" s="3">
-        <v>18.690000000000001</v>
+        <v>0.04</v>
       </c>
       <c r="H39" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="B40" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C40" t="s">
-        <v>15</v>
-      </c>
-      <c r="D40" t="s">
-        <v>38</v>
+        <v>9</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="E40" t="s">
-        <v>10</v>
-      </c>
-      <c r="F40" s="1">
-        <v>7.9480000000000004</v>
-      </c>
-      <c r="H40" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.5">
+        <v>13</v>
+      </c>
+      <c r="F40" s="3">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -2054,19 +2042,19 @@
         <v>44</v>
       </c>
       <c r="C41" t="s">
-        <v>15</v>
-      </c>
-      <c r="D41" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>60</v>
       </c>
       <c r="E41" t="s">
         <v>13</v>
       </c>
-      <c r="F41">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="F41" s="3">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -2074,173 +2062,135 @@
         <v>44</v>
       </c>
       <c r="C42" t="s">
-        <v>9</v>
-      </c>
-      <c r="D42" t="s">
-        <v>59</v>
+        <v>45</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="E42" t="s">
         <v>13</v>
       </c>
-      <c r="F42">
-        <v>0.04</v>
-      </c>
-      <c r="H42" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="F42" s="3">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C43" t="s">
         <v>9</v>
       </c>
-      <c r="D43" t="s">
-        <v>63</v>
+      <c r="D43" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="E43" t="s">
         <v>13</v>
       </c>
-      <c r="F43">
-        <v>0.28000000000000003</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.5">
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C44" t="s">
         <v>9</v>
       </c>
-      <c r="D44" t="s">
-        <v>61</v>
+      <c r="D44" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="E44" t="s">
         <v>13</v>
       </c>
-      <c r="F44">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.5">
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C45" t="s">
-        <v>45</v>
-      </c>
-      <c r="D45" t="s">
-        <v>62</v>
+        <v>9</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="E45" t="s">
         <v>13</v>
       </c>
-      <c r="F45">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.5">
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>46</v>
+      </c>
       <c r="B46" t="s">
         <v>46</v>
       </c>
       <c r="C46" t="s">
         <v>9</v>
       </c>
-      <c r="D46" t="s">
-        <v>49</v>
+      <c r="D46" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="E46" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
       <c r="B47" t="s">
         <v>46</v>
       </c>
       <c r="C47" t="s">
         <v>9</v>
       </c>
-      <c r="D47" t="s">
-        <v>50</v>
+      <c r="D47" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="E47" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="G47" t="s">
+        <v>48</v>
+      </c>
+      <c r="H47" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>46</v>
+      </c>
       <c r="B48" t="s">
         <v>46</v>
       </c>
       <c r="C48" t="s">
         <v>9</v>
       </c>
-      <c r="D48" t="s">
-        <v>51</v>
+      <c r="D48" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="E48" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.5">
-      <c r="B49" t="s">
-        <v>46</v>
-      </c>
-      <c r="C49" t="s">
-        <v>9</v>
-      </c>
-      <c r="D49" t="s">
-        <v>52</v>
-      </c>
-      <c r="E49" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.5">
-      <c r="B50" t="s">
-        <v>46</v>
-      </c>
-      <c r="C50" t="s">
-        <v>9</v>
-      </c>
-      <c r="D50" t="s">
-        <v>47</v>
-      </c>
-      <c r="E50" t="s">
-        <v>13</v>
-      </c>
-      <c r="G50" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.5">
-      <c r="B51" t="s">
-        <v>46</v>
-      </c>
-      <c r="C51" t="s">
-        <v>9</v>
-      </c>
-      <c r="D51" t="s">
-        <v>65</v>
-      </c>
-      <c r="E51" t="s">
-        <v>13</v>
+      <c r="H48" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H49">
-    <sortCondition ref="A2:A49"/>
-    <sortCondition ref="D2:D49"/>
-    <sortCondition ref="E2:E49"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H47">
+    <sortCondition ref="A2:A47"/>
+    <sortCondition ref="B2:B47"/>
+    <sortCondition ref="D2:D47"/>
+    <sortCondition ref="E2:E47"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Created 3 new zoop data files: zoop_month, zoop_annual_noregions, and zoop_annual_regions
</commit_message>
<xml_diff>
--- a/data/data_in/Zoop Categories for SEM.xlsx
+++ b/data/data_in/Zoop Categories for SEM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\NCEAS Working Group\Food Web Group\swg-21-foodwebs\data\data_in\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\swg-21-foodwebs\data\data_in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF49607-9317-4D0D-B8CA-DAF0E8B2EE75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FF0B0F-5268-409C-8E34-0ABD61D963A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zoop Categories for SEM" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="67">
   <si>
     <t>SEM Category</t>
   </si>
@@ -157,9 +157,6 @@
     <t>Omnivorous, mostly predatory</t>
   </si>
   <si>
-    <t>Hyperacanthomysis longirostorus</t>
-  </si>
-  <si>
     <t>Omnivores, suspension feeding?</t>
   </si>
   <si>
@@ -232,7 +229,7 @@
     <t>Pseudodiaptomus</t>
   </si>
   <si>
-    <t>Pseudodiaptomus spp.</t>
+    <t>Hyperacanthomysis longirostris</t>
   </si>
 </sst>
 </file>
@@ -1109,7 +1106,7 @@
   <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,7 +1144,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1170,7 +1167,7 @@
         <v>0.6</v>
       </c>
       <c r="H2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1193,7 +1190,7 @@
         <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1216,7 +1213,7 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1239,7 +1236,7 @@
         <v>2.98</v>
       </c>
       <c r="H5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1262,7 +1259,7 @@
         <v>1.3</v>
       </c>
       <c r="H6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1285,7 +1282,7 @@
         <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1308,7 +1305,7 @@
         <v>2</v>
       </c>
       <c r="H8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1331,7 +1328,7 @@
         <v>3.55</v>
       </c>
       <c r="H9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1354,7 +1351,7 @@
         <v>1.4430000000000001</v>
       </c>
       <c r="H10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1377,7 +1374,7 @@
         <v>0.1</v>
       </c>
       <c r="H11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1391,7 +1388,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E12" t="s">
         <v>20</v>
@@ -1400,7 +1397,7 @@
         <v>0.1</v>
       </c>
       <c r="H12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1423,7 +1420,7 @@
         <v>2.66</v>
       </c>
       <c r="H13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1446,7 +1443,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="H14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1460,7 +1457,7 @@
         <v>9</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1469,7 +1466,7 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="H15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1492,7 +1489,7 @@
         <v>3.4129999999999998</v>
       </c>
       <c r="H16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1515,7 +1512,7 @@
         <v>1.8109999999999999</v>
       </c>
       <c r="H17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1538,7 +1535,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1561,7 +1558,7 @@
         <v>3.8</v>
       </c>
       <c r="H19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1575,7 +1572,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E20" t="s">
         <v>20</v>
@@ -1604,7 +1601,7 @@
         <v>0.13300000000000001</v>
       </c>
       <c r="H21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1627,7 +1624,7 @@
         <v>0.04</v>
       </c>
       <c r="H22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1650,7 +1647,7 @@
         <v>0.02</v>
       </c>
       <c r="H23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1673,7 +1670,7 @@
         <v>0.13300000000000001</v>
       </c>
       <c r="H24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1696,7 +1693,7 @@
         <v>8.8663037E-2</v>
       </c>
       <c r="H25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1727,17 +1724,17 @@
         <v>15</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="E27" t="s">
         <v>13</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1761,7 +1758,7 @@
         <v>41</v>
       </c>
       <c r="H28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1784,7 +1781,7 @@
         <v>2.6659999999999999</v>
       </c>
       <c r="H29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1807,7 +1804,7 @@
         <v>1.1619999999999999</v>
       </c>
       <c r="H30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1830,7 +1827,7 @@
         <v>15.89</v>
       </c>
       <c r="H31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1853,7 +1850,7 @@
         <v>7.9480000000000004</v>
       </c>
       <c r="H32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1876,7 +1873,7 @@
         <v>3.36</v>
       </c>
       <c r="H33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1890,7 +1887,7 @@
         <v>15</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E34" t="s">
         <v>13</v>
@@ -1899,7 +1896,7 @@
         <v>0.20100000000000001</v>
       </c>
       <c r="H34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1913,7 +1910,7 @@
         <v>15</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E35" t="s">
         <v>10</v>
@@ -1922,7 +1919,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="H35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1945,7 +1942,7 @@
         <v>0.21</v>
       </c>
       <c r="H36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1968,21 +1965,21 @@
         <v>0.5</v>
       </c>
       <c r="H37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C38" t="s">
         <v>15</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E38" t="s">
         <v>13</v>
@@ -1993,16 +1990,16 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C39" t="s">
         <v>9</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E39" t="s">
         <v>13</v>
@@ -2011,21 +2008,21 @@
         <v>0.04</v>
       </c>
       <c r="H39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C40" t="s">
         <v>9</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E40" t="s">
         <v>13</v>
@@ -2036,16 +2033,16 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C41" t="s">
         <v>9</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E41" t="s">
         <v>13</v>
@@ -2056,16 +2053,16 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" t="s">
         <v>44</v>
       </c>
-      <c r="B42" t="s">
-        <v>44</v>
-      </c>
-      <c r="C42" t="s">
-        <v>45</v>
-      </c>
       <c r="D42" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E42" t="s">
         <v>13</v>
@@ -2076,16 +2073,16 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C43" t="s">
         <v>9</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E43" t="s">
         <v>13</v>
@@ -2093,16 +2090,16 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C44" t="s">
         <v>9</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E44" t="s">
         <v>13</v>
@@ -2110,16 +2107,16 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C45" t="s">
         <v>9</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E45" t="s">
         <v>13</v>
@@ -2127,16 +2124,16 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C46" t="s">
         <v>9</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E46" t="s">
         <v>13</v>
@@ -2144,45 +2141,45 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B47" t="s">
-        <v>46</v>
-      </c>
-      <c r="C47" t="s">
-        <v>9</v>
-      </c>
-      <c r="D47" s="1" t="s">
+      <c r="E47" t="s">
+        <v>13</v>
+      </c>
+      <c r="G47" t="s">
         <v>47</v>
       </c>
-      <c r="E47" t="s">
-        <v>13</v>
-      </c>
-      <c r="G47" t="s">
-        <v>48</v>
-      </c>
       <c r="H47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C48" t="s">
         <v>9</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E48" t="s">
         <v>13</v>
       </c>
       <c r="H48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding unid cladocerans and Synchaeta bicornis (rotifer) to zoop data
</commit_message>
<xml_diff>
--- a/data/data_in/Zoop Categories for SEM.xlsx
+++ b/data/data_in/Zoop Categories for SEM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\swg-21-foodwebs\data\data_in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FF0B0F-5268-409C-8E34-0ABD61D963A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609DEC78-B852-405E-858E-6F3048B8AD7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="0" windowWidth="38370" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zoop Categories for SEM" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="69">
   <si>
     <t>SEM Category</t>
   </si>
@@ -230,6 +230,12 @@
   </si>
   <si>
     <t>Hyperacanthomysis longirostris</t>
+  </si>
+  <si>
+    <t>Cladocera</t>
+  </si>
+  <si>
+    <t>Synchaeta bicornis</t>
   </si>
 </sst>
 </file>
@@ -1103,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,25 +1224,25 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="3">
-        <v>2.98</v>
+        <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1253,13 +1259,13 @@
         <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F6" s="3">
-        <v>1.3</v>
+        <v>2.98</v>
       </c>
       <c r="H6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1273,16 +1279,16 @@
         <v>9</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F7" s="3">
-        <v>4</v>
+        <v>1.3</v>
       </c>
       <c r="H7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1299,10 +1305,10 @@
         <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F8" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H8" t="s">
         <v>55</v>
@@ -1319,16 +1325,16 @@
         <v>9</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F9" s="3">
-        <v>3.55</v>
+        <v>2</v>
       </c>
       <c r="H9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1345,10 +1351,10 @@
         <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F10" s="3">
-        <v>1.4430000000000001</v>
+        <v>3.55</v>
       </c>
       <c r="H10" t="s">
         <v>54</v>
@@ -1368,10 +1374,10 @@
         <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F11" s="3">
-        <v>0.1</v>
+        <v>1.4430000000000001</v>
       </c>
       <c r="H11" t="s">
         <v>54</v>
@@ -1388,7 +1394,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
         <v>20</v>
@@ -1411,13 +1417,13 @@
         <v>9</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="4">
-        <v>2.66</v>
+        <v>20</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.1</v>
       </c>
       <c r="H13" t="s">
         <v>54</v>
@@ -1434,16 +1440,16 @@
         <v>9</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E14" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="3">
-        <v>4.9000000000000004</v>
+      <c r="F14" s="4">
+        <v>2.66</v>
       </c>
       <c r="H14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1457,16 +1463,16 @@
         <v>9</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F15" s="3">
-        <v>1.1499999999999999</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="H15" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1480,16 +1486,16 @@
         <v>9</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F16" s="3">
-        <v>3.4129999999999998</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="H16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1506,10 +1512,10 @@
         <v>37</v>
       </c>
       <c r="E17" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F17" s="3">
-        <v>1.8109999999999999</v>
+        <v>3.4129999999999998</v>
       </c>
       <c r="H17" t="s">
         <v>55</v>
@@ -1529,10 +1535,10 @@
         <v>37</v>
       </c>
       <c r="E18" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F18" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>1.8109999999999999</v>
       </c>
       <c r="H18" t="s">
         <v>55</v>
@@ -1543,22 +1549,22 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="E19" t="s">
         <v>20</v>
       </c>
       <c r="F19" s="3">
-        <v>3.8</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1566,19 +1572,22 @@
         <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>62</v>
+        <v>19</v>
       </c>
       <c r="E20" t="s">
         <v>20</v>
       </c>
       <c r="F20" s="3">
-        <v>0.1</v>
+        <v>3.8</v>
+      </c>
+      <c r="H20" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1586,22 +1595,19 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F21" s="3">
-        <v>0.13300000000000001</v>
-      </c>
-      <c r="H21" t="s">
-        <v>54</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1618,10 +1624,10 @@
         <v>30</v>
       </c>
       <c r="E22" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F22" s="3">
-        <v>0.04</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="H22" t="s">
         <v>54</v>
@@ -1641,10 +1647,10 @@
         <v>30</v>
       </c>
       <c r="E23" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" s="5">
-        <v>0.02</v>
+        <v>10</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0.04</v>
       </c>
       <c r="H23" t="s">
         <v>54</v>
@@ -1661,13 +1667,13 @@
         <v>9</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
-      </c>
-      <c r="F24" s="3">
-        <v>0.13300000000000001</v>
+        <v>20</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0.02</v>
       </c>
       <c r="H24" t="s">
         <v>54</v>
@@ -1684,13 +1690,13 @@
         <v>9</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E25" t="s">
         <v>13</v>
       </c>
       <c r="F25" s="3">
-        <v>8.8663037E-2</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="H25" t="s">
         <v>54</v>
@@ -1701,40 +1707,39 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E26" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="F26" s="3">
-        <v>1</v>
+        <v>8.8663037E-2</v>
+      </c>
+      <c r="H26" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="E27" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" s="3"/>
-      <c r="G27" t="s">
-        <v>42</v>
-      </c>
-      <c r="H27" t="s">
-        <v>54</v>
+        <v>27</v>
+      </c>
+      <c r="F27" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1748,14 +1753,14 @@
         <v>15</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="E28" t="s">
         <v>13</v>
       </c>
-      <c r="F28" s="5"/>
+      <c r="F28" s="3"/>
       <c r="G28" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H28" t="s">
         <v>54</v>
@@ -1763,22 +1768,23 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="C29" t="s">
         <v>15</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="E29" t="s">
         <v>13</v>
       </c>
-      <c r="F29" s="3">
-        <v>2.6659999999999999</v>
+      <c r="F29" s="5"/>
+      <c r="G29" t="s">
+        <v>41</v>
       </c>
       <c r="H29" t="s">
         <v>54</v>
@@ -1798,10 +1804,10 @@
         <v>16</v>
       </c>
       <c r="E30" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F30" s="3">
-        <v>1.1619999999999999</v>
+        <v>2.6659999999999999</v>
       </c>
       <c r="H30" t="s">
         <v>54</v>
@@ -1818,16 +1824,16 @@
         <v>15</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F31" s="4">
-        <v>15.89</v>
+        <v>10</v>
+      </c>
+      <c r="F31" s="3">
+        <v>1.1619999999999999</v>
       </c>
       <c r="H31" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1844,10 +1850,10 @@
         <v>38</v>
       </c>
       <c r="E32" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" s="6">
-        <v>7.9480000000000004</v>
+        <v>13</v>
+      </c>
+      <c r="F32" s="4">
+        <v>15.89</v>
       </c>
       <c r="H32" t="s">
         <v>56</v>
@@ -1858,22 +1864,22 @@
         <v>14</v>
       </c>
       <c r="B33" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C33" t="s">
         <v>15</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="E33" t="s">
-        <v>13</v>
-      </c>
-      <c r="F33" s="3">
-        <v>3.36</v>
+        <v>10</v>
+      </c>
+      <c r="F33" s="6">
+        <v>7.9480000000000004</v>
       </c>
       <c r="H33" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1887,16 +1893,16 @@
         <v>15</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="E34" t="s">
         <v>13</v>
       </c>
       <c r="F34" s="3">
-        <v>0.20100000000000001</v>
+        <v>3.36</v>
       </c>
       <c r="H34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1913,10 +1919,10 @@
         <v>64</v>
       </c>
       <c r="E35" t="s">
-        <v>10</v>
-      </c>
-      <c r="F35" s="5">
-        <v>6.6000000000000003E-2</v>
+        <v>13</v>
+      </c>
+      <c r="F35" s="3">
+        <v>0.20100000000000001</v>
       </c>
       <c r="H35" t="s">
         <v>56</v>
@@ -1933,13 +1939,13 @@
         <v>15</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="E36" t="s">
-        <v>13</v>
-      </c>
-      <c r="F36" s="3">
-        <v>0.21</v>
+        <v>10</v>
+      </c>
+      <c r="F36" s="5">
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="H36" t="s">
         <v>56</v>
@@ -1956,13 +1962,13 @@
         <v>15</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E37" t="s">
         <v>13</v>
       </c>
       <c r="F37" s="3">
-        <v>0.5</v>
+        <v>0.21</v>
       </c>
       <c r="H37" t="s">
         <v>56</v>
@@ -1970,22 +1976,25 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C38" t="s">
         <v>15</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="E38" t="s">
         <v>13</v>
       </c>
       <c r="F38" s="3">
-        <v>0.3</v>
+        <v>0.5</v>
+      </c>
+      <c r="H38" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1996,19 +2005,16 @@
         <v>43</v>
       </c>
       <c r="C39" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E39" t="s">
         <v>13</v>
       </c>
       <c r="F39" s="3">
-        <v>0.04</v>
-      </c>
-      <c r="H39" t="s">
-        <v>54</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -2022,13 +2028,16 @@
         <v>9</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E40" t="s">
         <v>13</v>
       </c>
       <c r="F40" s="3">
-        <v>0.28000000000000003</v>
+        <v>0.04</v>
+      </c>
+      <c r="H40" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -2042,13 +2051,13 @@
         <v>9</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E41" t="s">
         <v>13</v>
       </c>
       <c r="F41" s="3">
-        <v>0.12</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -2059,10 +2068,10 @@
         <v>43</v>
       </c>
       <c r="C42" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E42" t="s">
         <v>13</v>
@@ -2073,36 +2082,42 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C43" t="s">
         <v>9</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="E43" t="s">
         <v>13</v>
+      </c>
+      <c r="F43" s="3">
+        <v>0.12</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="E44" t="s">
         <v>13</v>
+      </c>
+      <c r="F44" s="3">
+        <v>0.12</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -2116,7 +2131,7 @@
         <v>9</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E45" t="s">
         <v>13</v>
@@ -2133,7 +2148,7 @@
         <v>9</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E46" t="s">
         <v>13</v>
@@ -2150,16 +2165,10 @@
         <v>9</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E47" t="s">
         <v>13</v>
-      </c>
-      <c r="G47" t="s">
-        <v>47</v>
-      </c>
-      <c r="H47" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -2173,21 +2182,61 @@
         <v>9</v>
       </c>
       <c r="D48" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E48" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E49" t="s">
+        <v>13</v>
+      </c>
+      <c r="G49" t="s">
+        <v>47</v>
+      </c>
+      <c r="H49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" t="s">
+        <v>45</v>
+      </c>
+      <c r="C50" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E48" t="s">
-        <v>13</v>
-      </c>
-      <c r="H48" t="s">
+      <c r="E50" t="s">
+        <v>13</v>
+      </c>
+      <c r="H50" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H47">
-    <sortCondition ref="A2:A47"/>
-    <sortCondition ref="B2:B47"/>
-    <sortCondition ref="D2:D47"/>
-    <sortCondition ref="E2:E47"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H49">
+    <sortCondition ref="A2:A49"/>
+    <sortCondition ref="B2:B49"/>
+    <sortCondition ref="D2:D49"/>
+    <sortCondition ref="E2:E49"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>